<commit_message>
Updating to allow for changing selectivity
</commit_message>
<xml_diff>
--- a/Data/CTL_parameters.xlsx
+++ b/Data/CTL_parameters.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michelle.Sculley\Documents\OpenScienceTraining\ISC_OSworkflow_training_dev\SS model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michelle.Sculley\Documents\SS_Intl_auto\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DE19875-2906-484B-9422-3E1BEDE0AF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F586B75D-4031-4EC0-BE76-64A9DAD24181}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2229" yWindow="2229" windowWidth="24685" windowHeight="13260" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SWO" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="951" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="975" uniqueCount="180">
   <si>
     <t>X1</t>
   </si>
@@ -557,13 +557,19 @@
   </si>
   <si>
     <t>LnQ_extraSD_2</t>
+  </si>
+  <si>
+    <t>SEL</t>
+  </si>
+  <si>
+    <t>DoubleNorm_F1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -599,8 +605,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -655,6 +666,12 @@
         <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor rgb="FFFFE599"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -668,7 +685,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
@@ -691,6 +708,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -915,7 +933,7 @@
       <selection sqref="A1:R75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -4755,15 +4773,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBB86EC-F98E-46C7-A441-180557FBE943}">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.45" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="26.07421875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.15234375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="14.6" x14ac:dyDescent="0.4">
@@ -4936,7 +4954,7 @@
         <v>0</v>
       </c>
       <c r="J4" s="5">
-        <v>4</v>
+        <v>-4</v>
       </c>
       <c r="K4" s="5">
         <v>0</v>
@@ -6448,8 +6466,8 @@
       <c r="A33" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>19</v>
+      <c r="B33" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>20</v>
@@ -6501,8 +6519,8 @@
       <c r="A34" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>19</v>
+      <c r="B34" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>20</v>
@@ -6554,8 +6572,8 @@
       <c r="A35" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>19</v>
+      <c r="B35" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>20</v>
@@ -6607,8 +6625,8 @@
       <c r="A36" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>19</v>
+      <c r="B36" s="18" t="s">
+        <v>178</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>20</v>
@@ -6656,7 +6674,432 @@
         <v>0</v>
       </c>
     </row>
+    <row r="37" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A37" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="B37" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D37" s="5">
+        <v>5</v>
+      </c>
+      <c r="E37" s="5">
+        <v>90</v>
+      </c>
+      <c r="F37" s="5">
+        <v>158.21899999999999</v>
+      </c>
+      <c r="G37" s="5">
+        <v>90</v>
+      </c>
+      <c r="H37" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="I37" s="5">
+        <v>0</v>
+      </c>
+      <c r="J37" s="5">
+        <v>2</v>
+      </c>
+      <c r="K37" s="5">
+        <v>0</v>
+      </c>
+      <c r="L37" s="5">
+        <v>0</v>
+      </c>
+      <c r="M37" s="5">
+        <v>0</v>
+      </c>
+      <c r="N37" s="5">
+        <v>0</v>
+      </c>
+      <c r="O37" s="5">
+        <v>0</v>
+      </c>
+      <c r="P37" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q37" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A38" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D38" s="5">
+        <v>-10</v>
+      </c>
+      <c r="E38" s="5">
+        <v>3</v>
+      </c>
+      <c r="F38" s="5">
+        <v>-7.6877199999999997</v>
+      </c>
+      <c r="G38" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H38" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="I38" s="5">
+        <v>0</v>
+      </c>
+      <c r="J38" s="5">
+        <v>3</v>
+      </c>
+      <c r="K38" s="5">
+        <v>0</v>
+      </c>
+      <c r="L38" s="5">
+        <v>0</v>
+      </c>
+      <c r="M38" s="5">
+        <v>0</v>
+      </c>
+      <c r="N38" s="5">
+        <v>0</v>
+      </c>
+      <c r="O38" s="5">
+        <v>0</v>
+      </c>
+      <c r="P38" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q38" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A39" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="B39" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D39" s="5">
+        <v>-4</v>
+      </c>
+      <c r="E39" s="5">
+        <v>12</v>
+      </c>
+      <c r="F39" s="5">
+        <v>7.6548499999999997</v>
+      </c>
+      <c r="G39" s="5">
+        <v>6</v>
+      </c>
+      <c r="H39" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="I39" s="5">
+        <v>0</v>
+      </c>
+      <c r="J39" s="5">
+        <v>3</v>
+      </c>
+      <c r="K39" s="5">
+        <v>0</v>
+      </c>
+      <c r="L39" s="5">
+        <v>0</v>
+      </c>
+      <c r="M39" s="5">
+        <v>0</v>
+      </c>
+      <c r="N39" s="5">
+        <v>0</v>
+      </c>
+      <c r="O39" s="5">
+        <v>0</v>
+      </c>
+      <c r="P39" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q39" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A40" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B40" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D40" s="5">
+        <v>-6</v>
+      </c>
+      <c r="E40" s="5">
+        <v>10</v>
+      </c>
+      <c r="F40" s="5">
+        <v>7.97471</v>
+      </c>
+      <c r="G40" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="H40" s="5">
+        <v>0.05</v>
+      </c>
+      <c r="I40" s="5">
+        <v>0</v>
+      </c>
+      <c r="J40" s="5">
+        <v>3</v>
+      </c>
+      <c r="K40" s="5">
+        <v>0</v>
+      </c>
+      <c r="L40" s="5">
+        <v>0</v>
+      </c>
+      <c r="M40" s="5">
+        <v>0</v>
+      </c>
+      <c r="N40" s="5">
+        <v>0</v>
+      </c>
+      <c r="O40" s="5">
+        <v>0</v>
+      </c>
+      <c r="P40" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q40" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A41" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B41" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D41" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E41" s="5">
+        <v>999</v>
+      </c>
+      <c r="F41" s="5">
+        <v>-999</v>
+      </c>
+      <c r="G41" s="5">
+        <v>-999</v>
+      </c>
+      <c r="H41" s="5">
+        <v>99</v>
+      </c>
+      <c r="I41" s="5">
+        <v>0</v>
+      </c>
+      <c r="J41" s="5">
+        <v>-2</v>
+      </c>
+      <c r="K41" s="5">
+        <v>0</v>
+      </c>
+      <c r="L41" s="5">
+        <v>0</v>
+      </c>
+      <c r="M41" s="5">
+        <v>0</v>
+      </c>
+      <c r="N41" s="5">
+        <v>0</v>
+      </c>
+      <c r="O41" s="5">
+        <v>0</v>
+      </c>
+      <c r="P41" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q41" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A42" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="B42" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D42" s="5">
+        <v>-999</v>
+      </c>
+      <c r="E42" s="5">
+        <v>999</v>
+      </c>
+      <c r="F42" s="5">
+        <v>-999</v>
+      </c>
+      <c r="G42" s="5">
+        <v>-999</v>
+      </c>
+      <c r="H42" s="5">
+        <v>99</v>
+      </c>
+      <c r="I42" s="5">
+        <v>0</v>
+      </c>
+      <c r="J42" s="5">
+        <v>-2</v>
+      </c>
+      <c r="K42" s="5">
+        <v>0</v>
+      </c>
+      <c r="L42" s="5">
+        <v>0</v>
+      </c>
+      <c r="M42" s="5">
+        <v>0</v>
+      </c>
+      <c r="N42" s="5">
+        <v>0</v>
+      </c>
+      <c r="O42" s="5">
+        <v>0</v>
+      </c>
+      <c r="P42" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q42" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A43" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="B43" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C43" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D43" s="5">
+        <v>19</v>
+      </c>
+      <c r="E43" s="5">
+        <v>70</v>
+      </c>
+      <c r="F43" s="5">
+        <v>36.659999999999997</v>
+      </c>
+      <c r="G43" s="5">
+        <v>30</v>
+      </c>
+      <c r="H43" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="I43" s="5">
+        <v>1</v>
+      </c>
+      <c r="J43" s="5">
+        <v>2</v>
+      </c>
+      <c r="K43" s="5">
+        <v>0</v>
+      </c>
+      <c r="L43" s="5">
+        <v>0</v>
+      </c>
+      <c r="M43" s="5">
+        <v>0</v>
+      </c>
+      <c r="N43" s="5">
+        <v>0</v>
+      </c>
+      <c r="O43" s="5">
+        <v>0</v>
+      </c>
+      <c r="P43" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q43" s="5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="14.6" x14ac:dyDescent="0.4">
+      <c r="A44" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="B44" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D44" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="E44" s="5">
+        <v>60</v>
+      </c>
+      <c r="F44" s="5">
+        <v>6.6</v>
+      </c>
+      <c r="G44" s="5">
+        <v>10</v>
+      </c>
+      <c r="H44" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="I44" s="5">
+        <v>1</v>
+      </c>
+      <c r="J44" s="5">
+        <v>3</v>
+      </c>
+      <c r="K44" s="5">
+        <v>0</v>
+      </c>
+      <c r="L44" s="5">
+        <v>0</v>
+      </c>
+      <c r="M44" s="5">
+        <v>0</v>
+      </c>
+      <c r="N44" s="5">
+        <v>0</v>
+      </c>
+      <c r="O44" s="5">
+        <v>0</v>
+      </c>
+      <c r="P44" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q44" s="5">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -6671,7 +7114,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:18" ht="14.6" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
@@ -11286,7 +11729,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.61328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="12.53515625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">

</xml_diff>